<commit_message>
Update DU for 28 SEP
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="44">
   <si>
     <t>Bug Log</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Successful login with incorrect username(case insensitive) and correct passowrd</t>
   </si>
   <si>
-    <t>Login page has undefined variable error</t>
-  </si>
-  <si>
     <t>Resolved</t>
   </si>
   <si>
@@ -146,6 +143,24 @@
   </si>
   <si>
     <t>Fixed</t>
+  </si>
+  <si>
+    <t>Login page has undefined variable 'error'</t>
+  </si>
+  <si>
+    <t>Login page displayed error message "A session had already been started"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biding </t>
+  </si>
+  <si>
+    <t>Biding page displayed syntax error, unexpected '}'</t>
+  </si>
+  <si>
+    <t>Admin(Bootstrap)</t>
+  </si>
+  <si>
+    <t>After browse and improt a zip file, page displayed synatx error message. Unexpected '}', expecting ';'.</t>
   </si>
 </sst>
 </file>
@@ -521,6 +536,49 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4466667</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>257071</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2476500" y="3048000"/>
+          <a:ext cx="4466667" cy="828571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -899,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -975,7 +1033,7 @@
       </c>
       <c r="G3" s="30">
         <f>SUM($F3:$F8)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H3" s="25" t="str">
         <f xml:space="preserve"> IF(G3&lt;10,Instructions!B7,Instructions!B8)</f>
@@ -993,7 +1051,7 @@
         <v>17</v>
       </c>
       <c r="D4" s="25" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>25</v>
@@ -1003,20 +1061,27 @@
       </c>
       <c r="G4" s="30"/>
       <c r="H4" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="21">
         <v>3</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="21">
+        <v>1</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>39</v>
+      </c>
       <c r="E5" s="21" t="s">
         <v>25</v>
       </c>
       <c r="F5" s="21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="30"/>
       <c r="H5" s="25"/>
@@ -1025,12 +1090,21 @@
       <c r="A6" s="21">
         <v>4</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="21">
+        <v>1</v>
+      </c>
+      <c r="C6" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>41</v>
+      </c>
       <c r="E6" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="21">
+        <v>1</v>
+      </c>
       <c r="G6" s="30"/>
       <c r="H6" s="25"/>
     </row>
@@ -1038,7 +1112,12 @@
       <c r="A7" s="21">
         <v>5</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="27">
+        <v>1</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>40</v>
+      </c>
       <c r="D7" s="26"/>
       <c r="E7" s="21" t="s">
         <v>25</v>
@@ -1109,12 +1188,17 @@
       <c r="G11" s="30"/>
       <c r="H11" s="25"/>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="21">
         <v>10</v>
       </c>
       <c r="B12" s="27"/>
-      <c r="C12" s="26"/>
+      <c r="C12" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>43</v>
+      </c>
       <c r="E12" s="21" t="s">
         <v>29</v>
       </c>
@@ -6415,6 +6499,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6422,8 +6507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6495,7 +6580,7 @@
         <v>Successful login with incorrect username(case insensitive) and correct passowrd</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="F3" s="29">
         <v>43732</v>
@@ -6518,10 +6603,10 @@
       </c>
       <c r="D4" s="10" t="str">
         <f>'Bug Metrics'!$D4</f>
-        <v>Login page has undefined variable error</v>
+        <v>Login page has undefined variable 'error'</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F4" s="29">
         <v>43732</v>
@@ -6530,7 +6615,7 @@
         <v>43733</v>
       </c>
       <c r="H4" s="19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -6540,15 +6625,15 @@
       </c>
       <c r="B5" s="9">
         <f>'Bug Metrics'!$B5</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="9">
+        <v>1</v>
+      </c>
+      <c r="C5" s="9" t="str">
         <f>'Bug Metrics'!$C5</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="10">
+        <v>Login (User)</v>
+      </c>
+      <c r="D5" s="10" t="str">
         <f>'Bug Metrics'!$D5</f>
-        <v>0</v>
+        <v>Login page displayed error message "A session had already been started"</v>
       </c>
       <c r="E5" s="11" t="s">
         <v>26</v>
@@ -6564,15 +6649,15 @@
       </c>
       <c r="B6" s="9">
         <f>'Bug Metrics'!$B6</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="C6" s="9" t="str">
         <f>'Bug Metrics'!$C6</f>
-        <v>0</v>
-      </c>
-      <c r="D6" s="10">
+        <v xml:space="preserve">Biding </v>
+      </c>
+      <c r="D6" s="10" t="str">
         <f>'Bug Metrics'!$D6</f>
-        <v>0</v>
+        <v>Biding page displayed syntax error, unexpected '}'</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>26</v>
@@ -6588,11 +6673,11 @@
       </c>
       <c r="B7" s="9">
         <f>'Bug Metrics'!$B7</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="str">
         <f>'Bug Metrics'!$C7</f>
-        <v>0</v>
+        <v xml:space="preserve">Biding </v>
       </c>
       <c r="D7" s="10">
         <f>'Bug Metrics'!$D7</f>
@@ -6709,9 +6794,9 @@
       <c r="C12" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="10">
+      <c r="D12" s="10" t="str">
         <f>'Bug Metrics'!$D12</f>
-        <v>0</v>
+        <v>After browse and improt a zip file, page displayed synatx error message. Unexpected '}', expecting ';'.</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Update DU for 1 October
</commit_message>
<xml_diff>
--- a/metrics/Bm.xlsx
+++ b/metrics/Bm.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
   <si>
     <t>Bug Log</t>
   </si>
@@ -160,16 +160,25 @@
     <t>Unable to validate userid with different casing in course_completed.csv</t>
   </si>
   <si>
-    <t>Unable to display error messages when importing SampleData(6 and 7).zip to validate bid.csv, although correct data imported to database</t>
-  </si>
-  <si>
-    <t>Biding (add bid)</t>
-  </si>
-  <si>
     <t>Unable to validate if student has not completed the prerequisite</t>
   </si>
   <si>
     <t>Unable to validate exam start and end time in course.csv (exam start time later than end time)</t>
+  </si>
+  <si>
+    <t>Unable to display error messages when importing SampleData(6 and 7).zip to validate bid.csv</t>
+  </si>
+  <si>
+    <t>Bidding (add bid)</t>
+  </si>
+  <si>
+    <t>Bidding(add bid)</t>
+  </si>
+  <si>
+    <t>When validating if student can add a bid with an incorrect course code, page displayed notice of 'Trying to get property 'school' of non-object'.</t>
+  </si>
+  <si>
+    <t>Unable to update bid amount when student bid twice for same section in the same round</t>
   </si>
 </sst>
 </file>
@@ -319,7 +328,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -394,6 +403,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -918,10 +930,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1001"/>
+  <dimension ref="A1:H1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -938,16 +950,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
     </row>
     <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
@@ -994,7 +1006,7 @@
       <c r="F3" s="19">
         <v>2</v>
       </c>
-      <c r="G3" s="29">
+      <c r="G3" s="30">
         <f>SUM($F3:$F6)</f>
         <v>5</v>
       </c>
@@ -1022,7 +1034,7 @@
       <c r="F4" s="19">
         <v>1</v>
       </c>
-      <c r="G4" s="29"/>
+      <c r="G4" s="30"/>
       <c r="H4" s="23" t="s">
         <v>33</v>
       </c>
@@ -1046,7 +1058,7 @@
       <c r="F5" s="19">
         <v>1</v>
       </c>
-      <c r="G5" s="29"/>
+      <c r="G5" s="30"/>
       <c r="H5" s="23"/>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1068,11 +1080,13 @@
       <c r="F6" s="19">
         <v>1</v>
       </c>
-      <c r="G6" s="29"/>
+      <c r="G6" s="30"/>
       <c r="H6" s="23"/>
     </row>
     <row r="7" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="28"/>
+      <c r="A7" s="28">
+        <v>5</v>
+      </c>
       <c r="B7" s="28">
         <v>1</v>
       </c>
@@ -1083,7 +1097,9 @@
       <c r="H7" s="23"/>
     </row>
     <row r="8" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="28"/>
+      <c r="A8" s="28">
+        <v>6</v>
+      </c>
       <c r="B8" s="28">
         <v>1</v>
       </c>
@@ -1112,9 +1128,9 @@
       <c r="F9" s="19">
         <v>1</v>
       </c>
-      <c r="G9" s="29">
-        <f>SUM(F9:F15)</f>
-        <v>14</v>
+      <c r="G9" s="30">
+        <f>SUM(F9:F18)</f>
+        <v>25</v>
       </c>
       <c r="H9" s="23" t="str">
         <f xml:space="preserve"> IF(G9&lt;10,Instructions!B7,Instructions!B8)</f>
@@ -1140,7 +1156,7 @@
       <c r="F10" s="19">
         <v>1</v>
       </c>
-      <c r="G10" s="29"/>
+      <c r="G10" s="30"/>
       <c r="H10" s="23"/>
     </row>
     <row r="11" spans="1:8" ht="45" x14ac:dyDescent="0.2">
@@ -1162,22 +1178,29 @@
       <c r="F11" s="19">
         <v>1</v>
       </c>
-      <c r="G11" s="29"/>
+      <c r="G11" s="30"/>
       <c r="H11" s="23"/>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="19">
         <v>10</v>
       </c>
       <c r="B12" s="25">
         <v>2</v>
       </c>
-      <c r="C12" s="24"/>
+      <c r="C12" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>45</v>
+      </c>
       <c r="E12" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="19"/>
-      <c r="G12" s="29"/>
+      <c r="F12" s="19">
+        <v>1</v>
+      </c>
+      <c r="G12" s="30"/>
       <c r="H12" s="23"/>
     </row>
     <row r="13" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1199,7 +1222,7 @@
       <c r="F13" s="19">
         <v>5</v>
       </c>
-      <c r="G13" s="29"/>
+      <c r="G13" s="30"/>
       <c r="H13" s="23"/>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -1213,7 +1236,7 @@
         <v>38</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E14" s="19" t="s">
         <v>26</v>
@@ -1221,7 +1244,7 @@
       <c r="F14" s="19">
         <v>5</v>
       </c>
-      <c r="G14" s="29"/>
+      <c r="G14" s="30"/>
       <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.2">
@@ -1232,18 +1255,18 @@
         <v>2</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E15" s="19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F15" s="19">
-        <v>1</v>
-      </c>
-      <c r="G15" s="29"/>
+        <v>5</v>
+      </c>
+      <c r="G15" s="30"/>
       <c r="H15" s="23"/>
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
@@ -1252,10 +1275,10 @@
         <v>2</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E16" s="28" t="s">
         <v>26</v>
@@ -1263,44 +1286,45 @@
       <c r="F16" s="28">
         <v>5</v>
       </c>
-      <c r="G16" s="28"/>
+      <c r="G16" s="30"/>
       <c r="H16" s="23"/>
     </row>
     <row r="17" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A17" s="19">
+      <c r="A17" s="29"/>
+      <c r="B17" s="25">
+        <v>2</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="29">
+        <v>1</v>
+      </c>
+      <c r="G17" s="30"/>
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="29"/>
+      <c r="B18" s="25">
+        <v>2</v>
+      </c>
+      <c r="C18" s="24"/>
+      <c r="E18" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="29"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="23"/>
+    </row>
+    <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="19">
         <v>14</v>
-      </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="24"/>
-      <c r="E17" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="29">
-        <f>SUM(F17:F20)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="23" t="str">
-        <f xml:space="preserve"> IF(G17&lt;10,Instructions!B7,Instructions!B8)</f>
-        <v>Use the planned debugging time in the iteration.</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="19">
-        <v>15</v>
-      </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="24"/>
-      <c r="E18" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="29"/>
-      <c r="H18" s="23"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="19">
-        <v>16</v>
       </c>
       <c r="B19" s="25"/>
       <c r="C19" s="24"/>
@@ -1308,12 +1332,18 @@
         <v>26</v>
       </c>
       <c r="F19" s="19"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="23"/>
+      <c r="G19" s="30">
+        <f>SUM(F19:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="23" t="str">
+        <f xml:space="preserve"> IF(G19&lt;10,Instructions!B7,Instructions!B8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B20" s="25"/>
       <c r="C20" s="24"/>
@@ -1321,31 +1351,25 @@
         <v>26</v>
       </c>
       <c r="F20" s="19"/>
-      <c r="G20" s="29"/>
+      <c r="G20" s="30"/>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="19">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="24"/>
       <c r="E21" s="19" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F21" s="19"/>
-      <c r="G21" s="29">
-        <f>SUM(F21:F24)</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="23" t="str">
-        <f xml:space="preserve"> IF(G21&lt;10,Instructions!B7,Instructions!B8)</f>
-        <v>Use the planned debugging time in the iteration.</v>
-      </c>
+      <c r="G21" s="30"/>
+      <c r="H21" s="23"/>
     </row>
     <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="24"/>
@@ -1353,12 +1377,12 @@
         <v>26</v>
       </c>
       <c r="F22" s="19"/>
-      <c r="G22" s="29"/>
+      <c r="G22" s="30"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" s="19">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B23" s="25"/>
       <c r="C23" s="24"/>
@@ -1366,96 +1390,106 @@
         <v>24</v>
       </c>
       <c r="F23" s="19"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="23"/>
+      <c r="G23" s="30">
+        <f>SUM(F23:F26)</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="23" t="str">
+        <f xml:space="preserve"> IF(G23&lt;10,Instructions!B7,Instructions!B8)</f>
+        <v>Use the planned debugging time in the iteration.</v>
+      </c>
     </row>
     <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="19">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B24" s="25"/>
       <c r="C24" s="24"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19" t="str">
-        <f>IF($E24="Critical", 10, IF($E24="High",5, IF($E24="Low",1,"")))</f>
-        <v/>
-      </c>
-      <c r="G24" s="29"/>
+      <c r="E24" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="30"/>
       <c r="H24" s="23"/>
     </row>
     <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="19">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="24"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19" t="str">
-        <f>IF($E25="Critical", 10, IF($E25="High",5, IF($E25="Low",1,"")))</f>
-        <v/>
-      </c>
+      <c r="E25" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="19"/>
+      <c r="G25" s="30"/>
+      <c r="H25" s="23"/>
     </row>
     <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="19">
-        <v>23</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B26" s="25"/>
+      <c r="C26" s="24"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19" t="str">
+        <f>IF($E26="Critical", 10, IF($E26="High",5, IF($E26="Low",1,"")))</f>
+        <v/>
+      </c>
+      <c r="G26" s="30"/>
+      <c r="H26" s="23"/>
     </row>
     <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="19">
-        <v>24</v>
+        <v>22</v>
+      </c>
+      <c r="B27" s="25"/>
+      <c r="C27" s="24"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19" t="str">
+        <f>IF($E27="Critical", 10, IF($E27="High",5, IF($E27="Low",1,"")))</f>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="19">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="19">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="19">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="19">
-        <v>28</v>
-      </c>
-      <c r="B31" s="25"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19" t="str">
-        <f t="shared" ref="F31:F201" si="0">IF($E31="Critical", 10, IF($E31="High",5, IF($E31="Low",1,"")))</f>
-        <v/>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="19">
-        <v>29</v>
-      </c>
-      <c r="B32" s="25"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <v>27</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="19">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B33" s="25"/>
       <c r="E33" s="19"/>
       <c r="F33" s="19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F33:F203" si="0">IF($E33="Critical", 10, IF($E33="High",5, IF($E33="Low",1,"")))</f>
         <v/>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="19">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B34" s="25"/>
       <c r="E34" s="19"/>
@@ -1466,7 +1500,7 @@
     </row>
     <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="19">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B35" s="25"/>
       <c r="E35" s="19"/>
@@ -1477,7 +1511,7 @@
     </row>
     <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="19">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B36" s="25"/>
       <c r="E36" s="19"/>
@@ -1488,7 +1522,7 @@
     </row>
     <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="19">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B37" s="25"/>
       <c r="E37" s="19"/>
@@ -1499,7 +1533,7 @@
     </row>
     <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="19">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B38" s="25"/>
       <c r="E38" s="19"/>
@@ -1510,7 +1544,7 @@
     </row>
     <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="19">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B39" s="25"/>
       <c r="E39" s="19"/>
@@ -1521,7 +1555,7 @@
     </row>
     <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="19">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B40" s="25"/>
       <c r="E40" s="19"/>
@@ -1532,7 +1566,7 @@
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="19">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B41" s="25"/>
       <c r="E41" s="19"/>
@@ -1543,7 +1577,7 @@
     </row>
     <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="19">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B42" s="25"/>
       <c r="E42" s="19"/>
@@ -1554,7 +1588,7 @@
     </row>
     <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="19">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B43" s="25"/>
       <c r="E43" s="19"/>
@@ -1565,7 +1599,7 @@
     </row>
     <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="19">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B44" s="25"/>
       <c r="E44" s="19"/>
@@ -1576,7 +1610,7 @@
     </row>
     <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="19">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B45" s="25"/>
       <c r="E45" s="19"/>
@@ -1587,7 +1621,7 @@
     </row>
     <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="19">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B46" s="25"/>
       <c r="E46" s="19"/>
@@ -1598,7 +1632,7 @@
     </row>
     <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="19">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B47" s="25"/>
       <c r="E47" s="19"/>
@@ -1609,7 +1643,7 @@
     </row>
     <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="19">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B48" s="25"/>
       <c r="E48" s="19"/>
@@ -1620,7 +1654,7 @@
     </row>
     <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="19">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B49" s="25"/>
       <c r="E49" s="19"/>
@@ -1631,7 +1665,7 @@
     </row>
     <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="19">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B50" s="25"/>
       <c r="E50" s="19"/>
@@ -1642,7 +1676,7 @@
     </row>
     <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="19">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B51" s="25"/>
       <c r="E51" s="19"/>
@@ -1653,7 +1687,7 @@
     </row>
     <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="19">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B52" s="25"/>
       <c r="E52" s="19"/>
@@ -1664,7 +1698,7 @@
     </row>
     <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="19">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B53" s="25"/>
       <c r="E53" s="19"/>
@@ -1675,7 +1709,7 @@
     </row>
     <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="19">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B54" s="25"/>
       <c r="E54" s="19"/>
@@ -1686,7 +1720,7 @@
     </row>
     <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="19">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B55" s="25"/>
       <c r="E55" s="19"/>
@@ -1697,7 +1731,7 @@
     </row>
     <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="19">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B56" s="25"/>
       <c r="E56" s="19"/>
@@ -1708,7 +1742,7 @@
     </row>
     <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="19">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B57" s="25"/>
       <c r="E57" s="19"/>
@@ -1719,7 +1753,7 @@
     </row>
     <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="19">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B58" s="25"/>
       <c r="E58" s="19"/>
@@ -1730,7 +1764,7 @@
     </row>
     <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="19">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B59" s="25"/>
       <c r="E59" s="19"/>
@@ -1741,7 +1775,7 @@
     </row>
     <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="19">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B60" s="25"/>
       <c r="E60" s="19"/>
@@ -1752,7 +1786,7 @@
     </row>
     <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="19">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B61" s="25"/>
       <c r="E61" s="19"/>
@@ -1763,7 +1797,7 @@
     </row>
     <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="19">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B62" s="25"/>
       <c r="E62" s="19"/>
@@ -1774,7 +1808,7 @@
     </row>
     <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="19">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B63" s="25"/>
       <c r="E63" s="19"/>
@@ -1785,7 +1819,7 @@
     </row>
     <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="19">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B64" s="25"/>
       <c r="E64" s="19"/>
@@ -1796,7 +1830,7 @@
     </row>
     <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="19">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B65" s="25"/>
       <c r="E65" s="19"/>
@@ -1807,7 +1841,7 @@
     </row>
     <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="19">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B66" s="25"/>
       <c r="E66" s="19"/>
@@ -1818,7 +1852,7 @@
     </row>
     <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="19">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B67" s="25"/>
       <c r="E67" s="19"/>
@@ -1829,7 +1863,7 @@
     </row>
     <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="19">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B68" s="25"/>
       <c r="E68" s="19"/>
@@ -1840,7 +1874,7 @@
     </row>
     <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="19">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B69" s="25"/>
       <c r="E69" s="19"/>
@@ -1851,7 +1885,7 @@
     </row>
     <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="19">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B70" s="25"/>
       <c r="E70" s="19"/>
@@ -1862,7 +1896,7 @@
     </row>
     <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="19">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B71" s="25"/>
       <c r="E71" s="19"/>
@@ -1873,7 +1907,7 @@
     </row>
     <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="19">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B72" s="25"/>
       <c r="E72" s="19"/>
@@ -1884,7 +1918,7 @@
     </row>
     <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="19">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B73" s="25"/>
       <c r="E73" s="19"/>
@@ -1895,7 +1929,7 @@
     </row>
     <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="19">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B74" s="25"/>
       <c r="E74" s="19"/>
@@ -1906,7 +1940,7 @@
     </row>
     <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="19">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B75" s="25"/>
       <c r="E75" s="19"/>
@@ -1917,7 +1951,7 @@
     </row>
     <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="19">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B76" s="25"/>
       <c r="E76" s="19"/>
@@ -1928,7 +1962,7 @@
     </row>
     <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="19">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B77" s="25"/>
       <c r="E77" s="19"/>
@@ -1939,7 +1973,7 @@
     </row>
     <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="19">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B78" s="25"/>
       <c r="E78" s="19"/>
@@ -1950,7 +1984,7 @@
     </row>
     <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="19">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B79" s="25"/>
       <c r="E79" s="19"/>
@@ -1961,7 +1995,7 @@
     </row>
     <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="19">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B80" s="25"/>
       <c r="E80" s="19"/>
@@ -1972,7 +2006,7 @@
     </row>
     <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="19">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B81" s="25"/>
       <c r="E81" s="19"/>
@@ -1983,7 +2017,7 @@
     </row>
     <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="19">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B82" s="25"/>
       <c r="E82" s="19"/>
@@ -1994,7 +2028,7 @@
     </row>
     <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="19">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B83" s="25"/>
       <c r="E83" s="19"/>
@@ -2005,7 +2039,7 @@
     </row>
     <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="19">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B84" s="25"/>
       <c r="E84" s="19"/>
@@ -2016,7 +2050,7 @@
     </row>
     <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="19">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B85" s="25"/>
       <c r="E85" s="19"/>
@@ -2027,7 +2061,7 @@
     </row>
     <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="19">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B86" s="25"/>
       <c r="E86" s="19"/>
@@ -2038,7 +2072,7 @@
     </row>
     <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="19">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B87" s="25"/>
       <c r="E87" s="19"/>
@@ -2049,7 +2083,7 @@
     </row>
     <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="19">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B88" s="25"/>
       <c r="E88" s="19"/>
@@ -2060,7 +2094,7 @@
     </row>
     <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="19">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B89" s="25"/>
       <c r="E89" s="19"/>
@@ -2071,7 +2105,7 @@
     </row>
     <row r="90" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="19">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B90" s="25"/>
       <c r="E90" s="19"/>
@@ -2082,7 +2116,7 @@
     </row>
     <row r="91" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="19">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B91" s="25"/>
       <c r="E91" s="19"/>
@@ -2093,7 +2127,7 @@
     </row>
     <row r="92" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="19">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B92" s="25"/>
       <c r="E92" s="19"/>
@@ -2104,7 +2138,7 @@
     </row>
     <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="19">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B93" s="25"/>
       <c r="E93" s="19"/>
@@ -2115,7 +2149,7 @@
     </row>
     <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="19">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B94" s="25"/>
       <c r="E94" s="19"/>
@@ -2126,7 +2160,7 @@
     </row>
     <row r="95" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="19">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B95" s="25"/>
       <c r="E95" s="19"/>
@@ -2137,7 +2171,7 @@
     </row>
     <row r="96" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="19">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B96" s="25"/>
       <c r="E96" s="19"/>
@@ -2148,7 +2182,7 @@
     </row>
     <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="19">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B97" s="25"/>
       <c r="E97" s="19"/>
@@ -2159,7 +2193,7 @@
     </row>
     <row r="98" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="19">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B98" s="25"/>
       <c r="E98" s="19"/>
@@ -2170,7 +2204,7 @@
     </row>
     <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="19">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B99" s="25"/>
       <c r="E99" s="19"/>
@@ -2181,7 +2215,7 @@
     </row>
     <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="19">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B100" s="25"/>
       <c r="E100" s="19"/>
@@ -2192,7 +2226,7 @@
     </row>
     <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="19">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B101" s="25"/>
       <c r="E101" s="19"/>
@@ -2203,7 +2237,7 @@
     </row>
     <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="19">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B102" s="25"/>
       <c r="E102" s="19"/>
@@ -2214,7 +2248,7 @@
     </row>
     <row r="103" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="19">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B103" s="25"/>
       <c r="E103" s="19"/>
@@ -2225,7 +2259,7 @@
     </row>
     <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="19">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B104" s="25"/>
       <c r="E104" s="19"/>
@@ -2236,7 +2270,7 @@
     </row>
     <row r="105" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="19">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B105" s="25"/>
       <c r="E105" s="19"/>
@@ -2247,7 +2281,7 @@
     </row>
     <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="19">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B106" s="25"/>
       <c r="E106" s="19"/>
@@ -2258,7 +2292,7 @@
     </row>
     <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="19">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B107" s="25"/>
       <c r="E107" s="19"/>
@@ -2269,7 +2303,7 @@
     </row>
     <row r="108" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="19">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B108" s="25"/>
       <c r="E108" s="19"/>
@@ -2280,7 +2314,7 @@
     </row>
     <row r="109" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="19">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B109" s="25"/>
       <c r="E109" s="19"/>
@@ -2291,7 +2325,7 @@
     </row>
     <row r="110" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="19">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B110" s="25"/>
       <c r="E110" s="19"/>
@@ -2302,7 +2336,7 @@
     </row>
     <row r="111" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="19">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B111" s="25"/>
       <c r="E111" s="19"/>
@@ -2313,7 +2347,7 @@
     </row>
     <row r="112" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="19">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B112" s="25"/>
       <c r="E112" s="19"/>
@@ -2324,7 +2358,7 @@
     </row>
     <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A113" s="19">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B113" s="25"/>
       <c r="E113" s="19"/>
@@ -2335,7 +2369,7 @@
     </row>
     <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A114" s="19">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B114" s="25"/>
       <c r="E114" s="19"/>
@@ -2346,7 +2380,7 @@
     </row>
     <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A115" s="19">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B115" s="25"/>
       <c r="E115" s="19"/>
@@ -2357,7 +2391,7 @@
     </row>
     <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A116" s="19">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B116" s="25"/>
       <c r="E116" s="19"/>
@@ -2368,7 +2402,7 @@
     </row>
     <row r="117" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A117" s="19">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B117" s="25"/>
       <c r="E117" s="19"/>
@@ -2379,7 +2413,7 @@
     </row>
     <row r="118" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A118" s="19">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B118" s="25"/>
       <c r="E118" s="19"/>
@@ -2390,7 +2424,7 @@
     </row>
     <row r="119" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A119" s="19">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B119" s="25"/>
       <c r="E119" s="19"/>
@@ -2401,7 +2435,7 @@
     </row>
     <row r="120" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A120" s="19">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B120" s="25"/>
       <c r="E120" s="19"/>
@@ -2412,7 +2446,7 @@
     </row>
     <row r="121" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A121" s="19">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B121" s="25"/>
       <c r="E121" s="19"/>
@@ -2423,7 +2457,7 @@
     </row>
     <row r="122" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A122" s="19">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B122" s="25"/>
       <c r="E122" s="19"/>
@@ -2434,7 +2468,7 @@
     </row>
     <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A123" s="19">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B123" s="25"/>
       <c r="E123" s="19"/>
@@ -2445,7 +2479,7 @@
     </row>
     <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A124" s="19">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B124" s="25"/>
       <c r="E124" s="19"/>
@@ -2456,7 +2490,7 @@
     </row>
     <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A125" s="19">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B125" s="25"/>
       <c r="E125" s="19"/>
@@ -2467,7 +2501,7 @@
     </row>
     <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A126" s="19">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B126" s="25"/>
       <c r="E126" s="19"/>
@@ -2478,7 +2512,7 @@
     </row>
     <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A127" s="19">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B127" s="25"/>
       <c r="E127" s="19"/>
@@ -2489,7 +2523,7 @@
     </row>
     <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A128" s="19">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B128" s="25"/>
       <c r="E128" s="19"/>
@@ -2500,7 +2534,7 @@
     </row>
     <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A129" s="19">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B129" s="25"/>
       <c r="E129" s="19"/>
@@ -2511,7 +2545,7 @@
     </row>
     <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A130" s="19">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B130" s="25"/>
       <c r="E130" s="19"/>
@@ -2522,7 +2556,7 @@
     </row>
     <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A131" s="19">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B131" s="25"/>
       <c r="E131" s="19"/>
@@ -2533,7 +2567,7 @@
     </row>
     <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A132" s="19">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B132" s="25"/>
       <c r="E132" s="19"/>
@@ -2544,7 +2578,7 @@
     </row>
     <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A133" s="19">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B133" s="25"/>
       <c r="E133" s="19"/>
@@ -2555,7 +2589,7 @@
     </row>
     <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A134" s="19">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B134" s="25"/>
       <c r="E134" s="19"/>
@@ -2566,7 +2600,7 @@
     </row>
     <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A135" s="19">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B135" s="25"/>
       <c r="E135" s="19"/>
@@ -2577,7 +2611,7 @@
     </row>
     <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A136" s="19">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B136" s="25"/>
       <c r="E136" s="19"/>
@@ -2588,7 +2622,7 @@
     </row>
     <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A137" s="19">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B137" s="25"/>
       <c r="E137" s="19"/>
@@ -2599,7 +2633,7 @@
     </row>
     <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A138" s="19">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B138" s="25"/>
       <c r="E138" s="19"/>
@@ -2610,7 +2644,7 @@
     </row>
     <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A139" s="19">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B139" s="25"/>
       <c r="E139" s="19"/>
@@ -2621,7 +2655,7 @@
     </row>
     <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A140" s="19">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B140" s="25"/>
       <c r="E140" s="19"/>
@@ -2632,7 +2666,7 @@
     </row>
     <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A141" s="19">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B141" s="25"/>
       <c r="E141" s="19"/>
@@ -2643,7 +2677,7 @@
     </row>
     <row r="142" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A142" s="19">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B142" s="25"/>
       <c r="E142" s="19"/>
@@ -2654,7 +2688,7 @@
     </row>
     <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A143" s="19">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B143" s="25"/>
       <c r="E143" s="19"/>
@@ -2665,7 +2699,7 @@
     </row>
     <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A144" s="19">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B144" s="25"/>
       <c r="E144" s="19"/>
@@ -2676,7 +2710,7 @@
     </row>
     <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A145" s="19">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B145" s="25"/>
       <c r="E145" s="19"/>
@@ -2687,7 +2721,7 @@
     </row>
     <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A146" s="19">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B146" s="25"/>
       <c r="E146" s="19"/>
@@ -2698,7 +2732,7 @@
     </row>
     <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A147" s="19">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B147" s="25"/>
       <c r="E147" s="19"/>
@@ -2709,7 +2743,7 @@
     </row>
     <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A148" s="19">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B148" s="25"/>
       <c r="E148" s="19"/>
@@ -2720,7 +2754,7 @@
     </row>
     <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A149" s="19">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B149" s="25"/>
       <c r="E149" s="19"/>
@@ -2731,7 +2765,7 @@
     </row>
     <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A150" s="19">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B150" s="25"/>
       <c r="E150" s="19"/>
@@ -2742,7 +2776,7 @@
     </row>
     <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A151" s="19">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B151" s="25"/>
       <c r="E151" s="19"/>
@@ -2753,7 +2787,7 @@
     </row>
     <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A152" s="19">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B152" s="25"/>
       <c r="E152" s="19"/>
@@ -2764,7 +2798,7 @@
     </row>
     <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A153" s="19">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B153" s="25"/>
       <c r="E153" s="19"/>
@@ -2775,7 +2809,7 @@
     </row>
     <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A154" s="19">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B154" s="25"/>
       <c r="E154" s="19"/>
@@ -2786,7 +2820,7 @@
     </row>
     <row r="155" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A155" s="19">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B155" s="25"/>
       <c r="E155" s="19"/>
@@ -2797,7 +2831,7 @@
     </row>
     <row r="156" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A156" s="19">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B156" s="25"/>
       <c r="E156" s="19"/>
@@ -2808,7 +2842,7 @@
     </row>
     <row r="157" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A157" s="19">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B157" s="25"/>
       <c r="E157" s="19"/>
@@ -2819,7 +2853,7 @@
     </row>
     <row r="158" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A158" s="19">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B158" s="25"/>
       <c r="E158" s="19"/>
@@ -2830,7 +2864,7 @@
     </row>
     <row r="159" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A159" s="19">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B159" s="25"/>
       <c r="E159" s="19"/>
@@ -2841,7 +2875,7 @@
     </row>
     <row r="160" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A160" s="19">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B160" s="25"/>
       <c r="E160" s="19"/>
@@ -2852,7 +2886,7 @@
     </row>
     <row r="161" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A161" s="19">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B161" s="25"/>
       <c r="E161" s="19"/>
@@ -2863,7 +2897,7 @@
     </row>
     <row r="162" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A162" s="19">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B162" s="25"/>
       <c r="E162" s="19"/>
@@ -2874,7 +2908,7 @@
     </row>
     <row r="163" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A163" s="19">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B163" s="25"/>
       <c r="E163" s="19"/>
@@ -2885,7 +2919,7 @@
     </row>
     <row r="164" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A164" s="19">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B164" s="25"/>
       <c r="E164" s="19"/>
@@ -2896,7 +2930,7 @@
     </row>
     <row r="165" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A165" s="19">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B165" s="25"/>
       <c r="E165" s="19"/>
@@ -2907,7 +2941,7 @@
     </row>
     <row r="166" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A166" s="19">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B166" s="25"/>
       <c r="E166" s="19"/>
@@ -2918,7 +2952,7 @@
     </row>
     <row r="167" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A167" s="19">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B167" s="25"/>
       <c r="E167" s="19"/>
@@ -2929,7 +2963,7 @@
     </row>
     <row r="168" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A168" s="19">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B168" s="25"/>
       <c r="E168" s="19"/>
@@ -2940,7 +2974,7 @@
     </row>
     <row r="169" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A169" s="19">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B169" s="25"/>
       <c r="E169" s="19"/>
@@ -2951,7 +2985,7 @@
     </row>
     <row r="170" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A170" s="19">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B170" s="25"/>
       <c r="E170" s="19"/>
@@ -2962,7 +2996,7 @@
     </row>
     <row r="171" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A171" s="19">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B171" s="25"/>
       <c r="E171" s="19"/>
@@ -2973,7 +3007,7 @@
     </row>
     <row r="172" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A172" s="19">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B172" s="25"/>
       <c r="E172" s="19"/>
@@ -2984,7 +3018,7 @@
     </row>
     <row r="173" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A173" s="19">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B173" s="25"/>
       <c r="E173" s="19"/>
@@ -2995,7 +3029,7 @@
     </row>
     <row r="174" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A174" s="19">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B174" s="25"/>
       <c r="E174" s="19"/>
@@ -3006,7 +3040,7 @@
     </row>
     <row r="175" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A175" s="19">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B175" s="25"/>
       <c r="E175" s="19"/>
@@ -3017,7 +3051,7 @@
     </row>
     <row r="176" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A176" s="19">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B176" s="25"/>
       <c r="E176" s="19"/>
@@ -3028,7 +3062,7 @@
     </row>
     <row r="177" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A177" s="19">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B177" s="25"/>
       <c r="E177" s="19"/>
@@ -3039,7 +3073,7 @@
     </row>
     <row r="178" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A178" s="19">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B178" s="25"/>
       <c r="E178" s="19"/>
@@ -3050,7 +3084,7 @@
     </row>
     <row r="179" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A179" s="19">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B179" s="25"/>
       <c r="E179" s="19"/>
@@ -3061,7 +3095,7 @@
     </row>
     <row r="180" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A180" s="19">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B180" s="25"/>
       <c r="E180" s="19"/>
@@ -3072,7 +3106,7 @@
     </row>
     <row r="181" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A181" s="19">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B181" s="25"/>
       <c r="E181" s="19"/>
@@ -3083,7 +3117,7 @@
     </row>
     <row r="182" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A182" s="19">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B182" s="25"/>
       <c r="E182" s="19"/>
@@ -3094,7 +3128,7 @@
     </row>
     <row r="183" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A183" s="19">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B183" s="25"/>
       <c r="E183" s="19"/>
@@ -3105,7 +3139,7 @@
     </row>
     <row r="184" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A184" s="19">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B184" s="25"/>
       <c r="E184" s="19"/>
@@ -3116,7 +3150,7 @@
     </row>
     <row r="185" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A185" s="19">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B185" s="25"/>
       <c r="E185" s="19"/>
@@ -3127,7 +3161,7 @@
     </row>
     <row r="186" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A186" s="19">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B186" s="25"/>
       <c r="E186" s="19"/>
@@ -3138,7 +3172,7 @@
     </row>
     <row r="187" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A187" s="19">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B187" s="25"/>
       <c r="E187" s="19"/>
@@ -3149,7 +3183,7 @@
     </row>
     <row r="188" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A188" s="19">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B188" s="25"/>
       <c r="E188" s="19"/>
@@ -3160,7 +3194,7 @@
     </row>
     <row r="189" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A189" s="19">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B189" s="25"/>
       <c r="E189" s="19"/>
@@ -3171,7 +3205,7 @@
     </row>
     <row r="190" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A190" s="19">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B190" s="25"/>
       <c r="E190" s="19"/>
@@ -3182,7 +3216,7 @@
     </row>
     <row r="191" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A191" s="19">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B191" s="25"/>
       <c r="E191" s="19"/>
@@ -3193,7 +3227,7 @@
     </row>
     <row r="192" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A192" s="19">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B192" s="25"/>
       <c r="E192" s="19"/>
@@ -3204,7 +3238,7 @@
     </row>
     <row r="193" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A193" s="19">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B193" s="25"/>
       <c r="E193" s="19"/>
@@ -3215,7 +3249,7 @@
     </row>
     <row r="194" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A194" s="19">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B194" s="25"/>
       <c r="E194" s="19"/>
@@ -3226,7 +3260,7 @@
     </row>
     <row r="195" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A195" s="19">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B195" s="25"/>
       <c r="E195" s="19"/>
@@ -3237,7 +3271,7 @@
     </row>
     <row r="196" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A196" s="19">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B196" s="25"/>
       <c r="E196" s="19"/>
@@ -3248,7 +3282,7 @@
     </row>
     <row r="197" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A197" s="19">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B197" s="25"/>
       <c r="E197" s="19"/>
@@ -3259,7 +3293,7 @@
     </row>
     <row r="198" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A198" s="19">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B198" s="25"/>
       <c r="E198" s="19"/>
@@ -3270,7 +3304,7 @@
     </row>
     <row r="199" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A199" s="19">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B199" s="25"/>
       <c r="E199" s="19"/>
@@ -3281,7 +3315,7 @@
     </row>
     <row r="200" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A200" s="19">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B200" s="25"/>
       <c r="E200" s="19"/>
@@ -3292,7 +3326,7 @@
     </row>
     <row r="201" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A201" s="19">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B201" s="25"/>
       <c r="E201" s="19"/>
@@ -3301,13 +3335,27 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A202" s="25"/>
+    <row r="202" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A202" s="19">
+        <v>197</v>
+      </c>
       <c r="B202" s="25"/>
-    </row>
-    <row r="203" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A203" s="25"/>
+      <c r="E202" s="19"/>
+      <c r="F202" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="203" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A203" s="19">
+        <v>198</v>
+      </c>
       <c r="B203" s="25"/>
+      <c r="E203" s="19"/>
+      <c r="F203" s="19" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
     <row r="204" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="25"/>
@@ -6501,13 +6549,21 @@
       <c r="A1001" s="25"/>
       <c r="B1001" s="25"/>
     </row>
+    <row r="1002" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1002" s="25"/>
+      <c r="B1002" s="25"/>
+    </row>
+    <row r="1003" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1003" s="25"/>
+      <c r="B1003" s="25"/>
+    </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="G21:G24"/>
-    <mergeCell ref="G17:G20"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="G19:G22"/>
     <mergeCell ref="G3:G6"/>
-    <mergeCell ref="G9:G15"/>
     <mergeCell ref="A1:H1"/>
+    <mergeCell ref="G9:G18"/>
   </mergeCells>
   <conditionalFormatting sqref="H1:H1048576">
     <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="Stop current Development">
@@ -6515,7 +6571,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" sqref="E31:E201 E3:E25">
+    <dataValidation type="list" allowBlank="1" sqref="E33:E203 E3:E27">
       <formula1>"Critical,High,Low"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6529,7 +6585,7 @@
   <dimension ref="A1:H998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6546,16 +6602,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
     </row>
     <row r="2" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
@@ -6775,7 +6831,7 @@
       <c r="G9" s="18"/>
       <c r="H9" s="17"/>
     </row>
-    <row r="10" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <f>'Bug Metrics'!$A11</f>
         <v>9</v>
@@ -6783,13 +6839,13 @@
       <c r="B10" s="9">
         <v>2</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="9" t="str">
         <f>'Bug Metrics'!$C12</f>
-        <v>0</v>
-      </c>
-      <c r="D10" s="10">
+        <v>Admin(Bootstrap)</v>
+      </c>
+      <c r="D10" s="10" t="str">
         <f>'Bug Metrics'!$D12</f>
-        <v>0</v>
+        <v>Unable to display error messages when importing SampleData(6 and 7).zip to validate bid.csv</v>
       </c>
       <c r="E10" s="11" t="s">
         <v>25</v>
@@ -6823,7 +6879,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="17"/>
     </row>
-    <row r="12" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <f>'Bug Metrics'!$A13</f>
         <v>11</v>
@@ -6858,11 +6914,11 @@
       </c>
       <c r="C13" s="9" t="str">
         <f>'Bug Metrics'!$C15</f>
-        <v>Admin(Bootstrap)</v>
+        <v>Bidding (add bid)</v>
       </c>
       <c r="D13" s="10" t="str">
         <f>'Bug Metrics'!$D15</f>
-        <v>Unable to display error messages when importing SampleData(6 and 7).zip to validate bid.csv, although correct data imported to database</v>
+        <v>Unable to update bid amount when student bid twice for same section in the same round</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>25</v>
@@ -6875,16 +6931,16 @@
     </row>
     <row r="14" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
-        <f>'Bug Metrics'!$A17</f>
+        <f>'Bug Metrics'!$A19</f>
         <v>14</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9">
-        <f>'Bug Metrics'!$C17</f>
+        <f>'Bug Metrics'!$C19</f>
         <v>0</v>
       </c>
       <c r="D14" s="10">
-        <f>'Bug Metrics'!$D17</f>
+        <f>'Bug Metrics'!$D19</f>
         <v>0</v>
       </c>
       <c r="E14" s="11" t="s">
@@ -6896,16 +6952,16 @@
     </row>
     <row r="15" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
-        <f>'Bug Metrics'!$A18</f>
+        <f>'Bug Metrics'!$A20</f>
         <v>15</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9">
-        <f>'Bug Metrics'!$C18</f>
+        <f>'Bug Metrics'!$C20</f>
         <v>0</v>
       </c>
       <c r="D15" s="10">
-        <f>'Bug Metrics'!$D18</f>
+        <f>'Bug Metrics'!$D20</f>
         <v>0</v>
       </c>
       <c r="E15" s="11" t="s">
@@ -6917,16 +6973,16 @@
     </row>
     <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
-        <f>'Bug Metrics'!$A19</f>
+        <f>'Bug Metrics'!$A21</f>
         <v>16</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9">
-        <f>'Bug Metrics'!$C19</f>
+        <f>'Bug Metrics'!$C21</f>
         <v>0</v>
       </c>
       <c r="D16" s="10">
-        <f>'Bug Metrics'!$D19</f>
+        <f>'Bug Metrics'!$D21</f>
         <v>0</v>
       </c>
       <c r="E16" s="11" t="s">
@@ -6938,16 +6994,16 @@
     </row>
     <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="9">
-        <f>'Bug Metrics'!$A20</f>
+        <f>'Bug Metrics'!$A22</f>
         <v>17</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9">
-        <f>'Bug Metrics'!$C20</f>
+        <f>'Bug Metrics'!$C22</f>
         <v>0</v>
       </c>
       <c r="D17" s="10">
-        <f>'Bug Metrics'!$D20</f>
+        <f>'Bug Metrics'!$D22</f>
         <v>0</v>
       </c>
       <c r="E17" s="11" t="s">
@@ -6959,19 +7015,19 @@
     </row>
     <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
-        <f>'Bug Metrics'!$A21</f>
+        <f>'Bug Metrics'!$A23</f>
         <v>18</v>
       </c>
       <c r="B18" s="9">
-        <f>'Bug Metrics'!$B21</f>
+        <f>'Bug Metrics'!$B23</f>
         <v>0</v>
       </c>
       <c r="C18" s="9">
-        <f>'Bug Metrics'!$C21</f>
+        <f>'Bug Metrics'!$C23</f>
         <v>0</v>
       </c>
       <c r="D18" s="10">
-        <f>'Bug Metrics'!$D21</f>
+        <f>'Bug Metrics'!$D23</f>
         <v>0</v>
       </c>
       <c r="E18" s="11" t="s">
@@ -6983,19 +7039,19 @@
     </row>
     <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
-        <f>'Bug Metrics'!$A22</f>
+        <f>'Bug Metrics'!$A24</f>
         <v>19</v>
       </c>
       <c r="B19" s="9">
-        <f>'Bug Metrics'!$B22</f>
+        <f>'Bug Metrics'!$B24</f>
         <v>0</v>
       </c>
       <c r="C19" s="9">
-        <f>'Bug Metrics'!$C22</f>
+        <f>'Bug Metrics'!$C24</f>
         <v>0</v>
       </c>
       <c r="D19" s="10">
-        <f>'Bug Metrics'!$D22</f>
+        <f>'Bug Metrics'!$D24</f>
         <v>0</v>
       </c>
       <c r="E19" s="11" t="s">
@@ -7007,19 +7063,19 @@
     </row>
     <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="9">
-        <f>'Bug Metrics'!$A23</f>
+        <f>'Bug Metrics'!$A25</f>
         <v>20</v>
       </c>
       <c r="B20" s="9">
-        <f>'Bug Metrics'!$B23</f>
+        <f>'Bug Metrics'!$B25</f>
         <v>0</v>
       </c>
       <c r="C20" s="9">
-        <f>'Bug Metrics'!$C23</f>
+        <f>'Bug Metrics'!$C25</f>
         <v>0</v>
       </c>
       <c r="D20" s="10">
-        <f>'Bug Metrics'!$D23</f>
+        <f>'Bug Metrics'!$D25</f>
         <v>0</v>
       </c>
       <c r="E20" s="11" t="s">
@@ -7031,19 +7087,19 @@
     </row>
     <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
-        <f>'Bug Metrics'!$A24</f>
+        <f>'Bug Metrics'!$A26</f>
         <v>21</v>
       </c>
       <c r="B21" s="9">
-        <f>'Bug Metrics'!$B24</f>
+        <f>'Bug Metrics'!$B26</f>
         <v>0</v>
       </c>
       <c r="C21" s="9">
-        <f>'Bug Metrics'!$C24</f>
+        <f>'Bug Metrics'!$C26</f>
         <v>0</v>
       </c>
       <c r="D21" s="10">
-        <f>'Bug Metrics'!$D24</f>
+        <f>'Bug Metrics'!$D26</f>
         <v>0</v>
       </c>
       <c r="E21" s="11" t="s">

</xml_diff>